<commit_message>
Windows Forms Resize haqqında Proyekt
</commit_message>
<xml_diff>
--- a/ExcelVTIntegrationProject/test.xlsx
+++ b/ExcelVTIntegrationProject/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Csharp-Sqlserver-Projects\ExcelVTIntegrationProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87D2D2C-3954-402D-949E-25AD50231FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C33D49-1F2B-477C-A962-CDDD8F6031B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>PersonalNo</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Barcelona</t>
+  </si>
+  <si>
+    <t>Pedri</t>
+  </si>
+  <si>
+    <t>Gonzales</t>
   </si>
 </sst>
 </file>
@@ -395,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" activeCellId="1" sqref="D3 G3"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +413,7 @@
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -424,9 +430,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>5</v>
@@ -441,9 +447,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
@@ -455,6 +461,23 @@
         <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>